<commit_message>
process renamed to protocol in many headers
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/current/filled/Q4DemoSS2Metadata_v5_plainHeaders_new.xlsx
+++ b/examples/spreadsheets/current/filled/Q4DemoSS2Metadata_v5_plainHeaders_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/Dropbox/HCA/preview_release_new_protocol_format/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/Google Drive/metadata-schema/examples/spreadsheets/current/filled/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{33483293-1C8F-8240-AF69-07B5EBAC9EBB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E23F8A6C-B8C0-F743-A880-914FCDD51C3F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="460" windowWidth="41840" windowHeight="21560" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9360" yWindow="460" windowWidth="41840" windowHeight="21560" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="431">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -1278,6 +1278,51 @@
   </si>
   <si>
     <t>single cell sequencing process</t>
+  </si>
+  <si>
+    <t>enrichment_protocol.protocol_core.protocol_name</t>
+  </si>
+  <si>
+    <t>enrichment_protocol.protocol_core.protocol_description</t>
+  </si>
+  <si>
+    <t>enrichment_protocol.protocol_core.start_time</t>
+  </si>
+  <si>
+    <t>enrichment_protocol.protocol_core.protocol_location</t>
+  </si>
+  <si>
+    <t>enrichment_protocol.protocol_core.operator_identity</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.protocol_core.protocol_name</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.protocol_core.protocol_description</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.protocol_core.start_time</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.protocol_core.protocol_location</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.protocol_core.operator_identity</t>
+  </si>
+  <si>
+    <t>sequencing_protocol.protocol_core.protocol_name</t>
+  </si>
+  <si>
+    <t>sequencing_protocol.protocol_core.protocol_description</t>
+  </si>
+  <si>
+    <t>sequencing_protocol.protocol_core.start_time</t>
+  </si>
+  <si>
+    <t>sequencing_protocol.protocol_core.protocol_location</t>
+  </si>
+  <si>
+    <t>sequencing_protocol.protocol_core.operator_identity</t>
   </si>
 </sst>
 </file>
@@ -1850,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3039,7 +3084,7 @@
   <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3331,8 +3376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3446,8 +3491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3527,19 +3572,19 @@
         <v>260</v>
       </c>
       <c r="B4" t="s">
-        <v>270</v>
+        <v>416</v>
       </c>
       <c r="C4" t="s">
-        <v>271</v>
+        <v>417</v>
       </c>
       <c r="D4" t="s">
-        <v>272</v>
+        <v>418</v>
       </c>
       <c r="E4" t="s">
-        <v>273</v>
+        <v>419</v>
       </c>
       <c r="F4" t="s">
-        <v>274</v>
+        <v>420</v>
       </c>
       <c r="G4" t="s">
         <v>275</v>
@@ -3588,8 +3633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AM6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AO4" sqref="AO4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3791,22 +3836,22 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>282</v>
+        <v>363</v>
       </c>
       <c r="B4" t="s">
-        <v>283</v>
+        <v>421</v>
       </c>
       <c r="C4" t="s">
-        <v>284</v>
+        <v>422</v>
       </c>
       <c r="D4" t="s">
-        <v>285</v>
+        <v>423</v>
       </c>
       <c r="E4" t="s">
-        <v>286</v>
+        <v>424</v>
       </c>
       <c r="F4" t="s">
-        <v>287</v>
+        <v>425</v>
       </c>
       <c r="G4" t="s">
         <v>288</v>
@@ -3942,8 +3987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4032,22 +4077,22 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>321</v>
+        <v>366</v>
       </c>
       <c r="B4" t="s">
-        <v>322</v>
+        <v>426</v>
       </c>
       <c r="C4" t="s">
-        <v>323</v>
+        <v>427</v>
       </c>
       <c r="D4" t="s">
-        <v>324</v>
+        <v>428</v>
       </c>
       <c r="E4" t="s">
-        <v>325</v>
+        <v>429</v>
       </c>
       <c r="F4" t="s">
-        <v>326</v>
+        <v>430</v>
       </c>
       <c r="G4" t="s">
         <v>327</v>
@@ -4065,7 +4110,7 @@
         <v>331</v>
       </c>
       <c r="L4" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="M4" t="s">
         <v>335</v>

</xml_diff>